<commit_message>
Added weight vs date graph program
The program opens up a window with the weight vs date graph, but it still needs to be integrated with the main program
</commit_message>
<xml_diff>
--- a/Current Patients/TeSt2/DataBases/Data/TeSt2_Anthropometrics_Source.xlsx
+++ b/Current Patients/TeSt2/DataBases/Data/TeSt2_Anthropometrics_Source.xlsx
@@ -399,10 +399,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U7"/>
+  <dimension ref="A1:U8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.75"/>
@@ -842,13 +842,13 @@
         <v>2</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7" t="n">
         <v>14</v>
       </c>
       <c r="F7" t="n">
-        <v>1.13</v>
+        <v>1</v>
       </c>
       <c r="G7" t="n">
         <v>1.1</v>
@@ -880,17 +880,79 @@
       <c r="P7" t="n">
         <v>1.1</v>
       </c>
-      <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="inlineStr"/>
       <c r="S7" t="inlineStr">
         <is>
           <t>RP-6/30/2020</t>
         </is>
       </c>
-      <c r="T7" t="inlineStr"/>
       <c r="U7" t="inlineStr">
         <is>
           <t>hi</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>2</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>7/1/2020</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" t="n">
+        <v>14</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="J8" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="K8" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="L8" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="M8" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="N8" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="O8" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="P8" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="Q8" t="inlineStr"/>
+      <c r="R8" t="inlineStr"/>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>RP-7/1/2020</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr"/>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>hello</t>
         </is>
       </c>
     </row>

</xml_diff>